<commit_message>
Modified Main to run 3 prediction methods in sequence
</commit_message>
<xml_diff>
--- a/UncertainRoadNetwork/Results/New Experiments/results_links_Interpolate_continuous3.xlsx
+++ b/UncertainRoadNetwork/Results/New Experiments/results_links_Interpolate_continuous3.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="results_links_Interpolate_conti" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1019,7 +1019,7 @@
   <dimension ref="A5:DV62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22323,35 +22323,21 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="DR8:DV8"/>
-    <mergeCell ref="CN8:CR8"/>
-    <mergeCell ref="CS8:CW8"/>
-    <mergeCell ref="CX8:DB8"/>
-    <mergeCell ref="DC8:DG8"/>
-    <mergeCell ref="DH8:DL8"/>
-    <mergeCell ref="DM8:DQ8"/>
-    <mergeCell ref="BJ8:BN8"/>
-    <mergeCell ref="BO8:BS8"/>
-    <mergeCell ref="BT8:BX8"/>
-    <mergeCell ref="BY8:CC8"/>
-    <mergeCell ref="CD8:CH8"/>
-    <mergeCell ref="CI8:CM8"/>
-    <mergeCell ref="AF8:AJ8"/>
-    <mergeCell ref="AK8:AO8"/>
-    <mergeCell ref="AP8:AT8"/>
-    <mergeCell ref="AU8:AY8"/>
-    <mergeCell ref="AZ8:BD8"/>
-    <mergeCell ref="BE8:BI8"/>
-    <mergeCell ref="B5:Z5"/>
-    <mergeCell ref="AA5:AY5"/>
-    <mergeCell ref="AZ5:BX5"/>
-    <mergeCell ref="BY5:CW5"/>
-    <mergeCell ref="CX5:DV5"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="V8:Z8"/>
-    <mergeCell ref="AA8:AE8"/>
+    <mergeCell ref="V7:Z7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="BT7:BX7"/>
+    <mergeCell ref="BY7:CC7"/>
+    <mergeCell ref="CD7:CH7"/>
+    <mergeCell ref="AA7:AE7"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AK7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="AU7:AY7"/>
+    <mergeCell ref="AZ7:BD7"/>
     <mergeCell ref="DM7:DQ7"/>
     <mergeCell ref="DR7:DV7"/>
     <mergeCell ref="CX6:DV6"/>
@@ -22368,21 +22354,35 @@
     <mergeCell ref="BE7:BI7"/>
     <mergeCell ref="BJ7:BN7"/>
     <mergeCell ref="BO7:BS7"/>
-    <mergeCell ref="BT7:BX7"/>
-    <mergeCell ref="BY7:CC7"/>
-    <mergeCell ref="CD7:CH7"/>
-    <mergeCell ref="AA7:AE7"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AK7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="AU7:AY7"/>
-    <mergeCell ref="AZ7:BD7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="V7:Z7"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="V8:Z8"/>
+    <mergeCell ref="AA8:AE8"/>
+    <mergeCell ref="B5:Z5"/>
+    <mergeCell ref="AA5:AY5"/>
+    <mergeCell ref="AZ5:BX5"/>
+    <mergeCell ref="BY5:CW5"/>
+    <mergeCell ref="CX5:DV5"/>
+    <mergeCell ref="CI8:CM8"/>
+    <mergeCell ref="AF8:AJ8"/>
+    <mergeCell ref="AK8:AO8"/>
+    <mergeCell ref="AP8:AT8"/>
+    <mergeCell ref="AU8:AY8"/>
+    <mergeCell ref="AZ8:BD8"/>
+    <mergeCell ref="BE8:BI8"/>
+    <mergeCell ref="BJ8:BN8"/>
+    <mergeCell ref="BO8:BS8"/>
+    <mergeCell ref="BT8:BX8"/>
+    <mergeCell ref="BY8:CC8"/>
+    <mergeCell ref="CD8:CH8"/>
+    <mergeCell ref="DR8:DV8"/>
+    <mergeCell ref="CN8:CR8"/>
+    <mergeCell ref="CS8:CW8"/>
+    <mergeCell ref="CX8:DB8"/>
+    <mergeCell ref="DC8:DG8"/>
+    <mergeCell ref="DH8:DL8"/>
+    <mergeCell ref="DM8:DQ8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>